<commit_message>
1/10 the way there
</commit_message>
<xml_diff>
--- a/src/FileCabinet/SuiteScripts/Consumption/Consumption Templates/Spice.xlsx
+++ b/src/FileCabinet/SuiteScripts/Consumption/Consumption Templates/Spice.xlsx
@@ -1,31 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\WebstormProjects\Spice Script\src\FileCabinet\SuiteScripts\Consumption\Consumption Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44B21E4-D2CD-4A89-871C-6A1F01E281EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40BEE7B-6AEC-4255-B7F1-62394B6D7DAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="main" sheetId="1" r:id="rId1"/>
+    <sheet name="lookup" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Internal Id</t>
   </si>
@@ -36,7 +46,13 @@
     <t>Item Description</t>
   </si>
   <si>
-    <t>H</t>
+    <t>Work Order Item</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Lot</t>
   </si>
 </sst>
 </file>
@@ -361,34 +377,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D2"/>
+  <dimension ref="A2:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.453125" customWidth="1"/>
+    <col min="6" max="6" width="18.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09059847-8055-48D2-A73C-F8CDCD0B3537}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="4.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>